<commit_message>
fixing error in get request
</commit_message>
<xml_diff>
--- a/pokemon/export_dataframe.xlsx
+++ b/pokemon/export_dataframe.xlsx
@@ -457,7 +457,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -473,7 +473,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -489,7 +489,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -505,7 +505,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -521,7 +521,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -537,7 +537,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -553,7 +553,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -569,7 +569,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -585,7 +585,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -601,7 +601,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -617,7 +617,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -633,7 +633,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -649,7 +649,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -665,7 +665,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -681,7 +681,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -697,7 +697,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -713,7 +713,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -729,7 +729,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -745,7 +745,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -761,7 +761,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1154</v>
+        <v>1279</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>

</xml_diff>